<commit_message>
Added total revenue chart
</commit_message>
<xml_diff>
--- a/PPF.xlsx
+++ b/PPF.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="1220" windowWidth="32460" windowHeight="21460" tabRatio="500"/>
+    <workbookView xWindow="2940" yWindow="1220" windowWidth="41820" windowHeight="22540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>La Famiglia Pizzeria and Bookstore</t>
   </si>
@@ -92,13 +92,21 @@
   <si>
     <t>Enter cost of 1 book:</t>
   </si>
+  <si>
+    <t>Pizza Possibilities:</t>
+  </si>
+  <si>
+    <t>Book Possibilities:</t>
+  </si>
+  <si>
+    <t>Tot. Revenue:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
@@ -147,7 +155,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -176,6 +184,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -187,7 +201,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -219,8 +233,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -229,30 +252,40 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="4"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="7" applyBorder="1"/>
+    <xf numFmtId="44" fontId="4" fillId="2" borderId="2" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="7" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="2" borderId="2" xfId="4" applyNumberFormat="1"/>
-    <xf numFmtId="8" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="6" borderId="0" xfId="8" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="9">
+    <cellStyle name="40% - Accent6" xfId="8" builtinId="51"/>
     <cellStyle name="Accent2" xfId="5" builtinId="33"/>
     <cellStyle name="Accent5" xfId="6" builtinId="45"/>
     <cellStyle name="Accent6" xfId="7" builtinId="49"/>
@@ -262,7 +295,28 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="2" builtinId="15"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -393,84 +447,84 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$9:$L$9</c:f>
+              <c:f>Sheet1!$B$12:$L$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>12.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.85226008714165</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.41267819554184</c:v>
+                  <c:v>7.950753362380551</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.69207829026041</c:v>
+                  <c:v>11.75497942756117</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.708203932499369</c:v>
+                  <c:v>15.31900552431464</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.48528137423857</c:v>
+                  <c:v>18.55507350181443</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.053423027509677</c:v>
+                  <c:v>21.38350062656062</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.447885996874561</c:v>
+                  <c:v>23.73464163573051</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.708203932499368</c:v>
+                  <c:v>25.5506036346887</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.87721358048277</c:v>
+                  <c:v>26.78667161218849</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.0</c:v>
+                  <c:v>27.41240947234941</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$10:$L$10</c:f>
+              <c:f>Sheet1!$B$13:$L$13</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>27.41240947234941</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26.78667161218849</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25.5506036346887</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23.73464163573051</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21.38350062656062</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18.55507350181443</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15.31900552431464</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.75497942756117</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.950753362380551</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.877213580482771</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.708203932499369</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.447885996874562</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7.053423027509677</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8.485281374238571</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>9.708203932499369</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>10.69207829026042</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>11.41267819554184</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>11.85226008714165</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>12.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -492,7 +546,8 @@
         <c:axId val="-2134385040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="14.0"/>
+          <c:max val="40.0"/>
+          <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -585,12 +640,13 @@
         <c:crossAx val="-2134580480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="8.0"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="-2134580480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="14.0"/>
+          <c:max val="40.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -688,6 +744,400 @@
         <c:crossAx val="-2134385040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="8.0"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Total Revenue</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$14:$L$14</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>274.1240947234941</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>315.8667161218849</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>350.9150766954536</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>378.4061694880391</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>397.6630725573818</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>408.2116170399174</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>409.7920627618738</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>402.3654939043778</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>386.1147772400699</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>361.4400593462619</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>328.948913668193</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="-1934518656"/>
+        <c:axId val="-2101366304"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-1934518656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Workers making Pizza (Added from Left to Right)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2101366304"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2101366304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1934518656"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -777,6 +1227,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
   <cs:axisTitle>
@@ -1315,20 +1805,569 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="236">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>19843</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>192086</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1964530</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>200023</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>325438</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>87312</xdr:rowOff>
+      <xdr:colOff>301625</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1342,6 +2381,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>11906</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>200024</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>456406</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1613,18 +2682,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:L10"/>
+  <dimension ref="A2:R14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.83203125" customWidth="1"/>
+    <col min="13" max="13" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" ht="24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="24" x14ac:dyDescent="0.3">
       <c r="D2" s="2" t="s">
         <v>15</v>
       </c>
@@ -1634,7 +2704,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="4" spans="1:12" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1644,163 +2714,309 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="6">
+        <v>4</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="12"/>
+      <c r="F6" s="7">
         <v>12</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="10">
+      <c r="H6" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="12"/>
+      <c r="J6" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" s="9"/>
-      <c r="J6" s="11">
-        <v>15</v>
+      <c r="K8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="5" t="s">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="5">
+        <f>B6</f>
         <v>4</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="L8" s="5" t="s">
-        <v>14</v>
+      <c r="C9" s="5">
+        <f>SIN(81 * PI() / 180) * B9</f>
+        <v>3.9507533623805511</v>
+      </c>
+      <c r="D9" s="5">
+        <f>SIN(72 * PI() / 180) * B9</f>
+        <v>3.8042260651806141</v>
+      </c>
+      <c r="E9" s="5">
+        <f>SIN(63 * PI() / 180) * B9</f>
+        <v>3.5640260967534712</v>
+      </c>
+      <c r="F9" s="5">
+        <f>SIN(54 * PI() / 180) * B9</f>
+        <v>3.2360679774997898</v>
+      </c>
+      <c r="G9" s="5">
+        <f>SIN(45 * PI() / 180) * B9</f>
+        <v>2.8284271247461898</v>
+      </c>
+      <c r="H9" s="5">
+        <f>SIN(36 * PI() / 180) * B9</f>
+        <v>2.3511410091698925</v>
+      </c>
+      <c r="I9" s="5">
+        <f>SIN(27 * PI() / 180) * B9</f>
+        <v>1.815961998958187</v>
+      </c>
+      <c r="J9" s="5">
+        <f>SIN(18 * PI() / 180) * B9</f>
+        <v>1.2360679774997896</v>
+      </c>
+      <c r="K9" s="5">
+        <f>SIN(9 * PI() / 180) * B9</f>
+        <v>0.62573786016092348</v>
+      </c>
+      <c r="L9" s="5">
+        <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="6">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="5">
+        <v>0</v>
+      </c>
+      <c r="C10" s="5">
+        <f>COS(81 * PI() / 180) * L10</f>
+        <v>0.6257378601609237</v>
+      </c>
+      <c r="D10" s="5">
+        <f>COS(72 * PI() / 180) * L10</f>
+        <v>1.2360679774997898</v>
+      </c>
+      <c r="E10" s="5">
+        <f>COS(63 * PI() / 180) * L10</f>
+        <v>1.8159619989581872</v>
+      </c>
+      <c r="F10" s="5">
+        <f>COS(54 * PI() / 180) * L10</f>
+        <v>2.3511410091698925</v>
+      </c>
+      <c r="G10" s="5">
+        <f>COS(45 * PI() / 180) * L10</f>
+        <v>2.8284271247461903</v>
+      </c>
+      <c r="H10" s="5">
+        <f>COS(36 * PI() / 180) * L10</f>
+        <v>3.2360679774997898</v>
+      </c>
+      <c r="I10" s="5">
+        <f>COS(27 * PI() / 180) * L10</f>
+        <v>3.5640260967534716</v>
+      </c>
+      <c r="J10" s="5">
+        <f>COS(18 * PI() / 180) * L10</f>
+        <v>3.8042260651806141</v>
+      </c>
+      <c r="K10" s="5">
+        <f>COS(9 * PI() / 180) * L10</f>
+        <v>3.9507533623805511</v>
+      </c>
+      <c r="L10" s="5">
         <f>B6</f>
-        <v>12</v>
-      </c>
-      <c r="C9" s="6">
-        <f>SIN(81 * PI() / 180) * B9</f>
-        <v>11.852260087141653</v>
-      </c>
-      <c r="D9" s="6">
-        <f>SIN(72 * PI() / 180) * B9</f>
-        <v>11.412678195541842</v>
-      </c>
-      <c r="E9" s="6">
-        <f>SIN(63 * PI() / 180) * B9</f>
-        <v>10.692078290260413</v>
-      </c>
-      <c r="F9" s="6">
-        <f>SIN(54 * PI() / 180) * B9</f>
-        <v>9.7082039324993694</v>
-      </c>
-      <c r="G9" s="6">
-        <f>SIN(45 * PI() / 180) * B9</f>
-        <v>8.4852813742385695</v>
-      </c>
-      <c r="H9" s="6">
-        <f>SIN(36 * PI() / 180) * B9</f>
-        <v>7.0534230275096776</v>
-      </c>
-      <c r="I9" s="6">
-        <f>SIN(27 * PI() / 180) * B9</f>
-        <v>5.447885996874561</v>
-      </c>
-      <c r="J9" s="6">
-        <f>SIN(18 * PI() / 180) * B9</f>
-        <v>3.7082039324993685</v>
-      </c>
-      <c r="K9" s="6">
-        <f>SIN(9 * PI() / 180) * B9</f>
-        <v>1.8772135804827705</v>
-      </c>
-      <c r="L9" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="5">
         <v>0</v>
       </c>
+      <c r="C12" s="5">
+        <f>B12+B9</f>
+        <v>4</v>
+      </c>
+      <c r="D12" s="5">
+        <f>C12+C9</f>
+        <v>7.9507533623805511</v>
+      </c>
+      <c r="E12" s="5">
+        <f>D12+D9</f>
+        <v>11.754979427561166</v>
+      </c>
+      <c r="F12" s="5">
+        <f>E12+E9</f>
+        <v>15.319005524314637</v>
+      </c>
+      <c r="G12" s="5">
+        <f>F12+F9</f>
+        <v>18.555073501814427</v>
+      </c>
+      <c r="H12" s="5">
+        <f>G12+G9</f>
+        <v>21.383500626560618</v>
+      </c>
+      <c r="I12" s="5">
+        <f>H12+H9</f>
+        <v>23.734641635730512</v>
+      </c>
+      <c r="J12" s="5">
+        <f>I12+I9</f>
+        <v>25.550603634688699</v>
+      </c>
+      <c r="K12" s="5">
+        <f>J12+J9</f>
+        <v>26.786671612188488</v>
+      </c>
+      <c r="L12" s="5">
+        <f>K12+K9</f>
+        <v>27.412409472349413</v>
+      </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="6">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="5">
+        <f>C13+C10</f>
+        <v>27.412409472349413</v>
+      </c>
+      <c r="C13" s="5">
+        <f>D13+D10</f>
+        <v>26.786671612188488</v>
+      </c>
+      <c r="D13" s="5">
+        <f>E13+E10</f>
+        <v>25.550603634688699</v>
+      </c>
+      <c r="E13" s="5">
+        <f>F13+F10</f>
+        <v>23.734641635730512</v>
+      </c>
+      <c r="F13" s="5">
+        <f>G13+G10</f>
+        <v>21.383500626560618</v>
+      </c>
+      <c r="G13" s="5">
+        <f>H13+H10</f>
+        <v>18.555073501814427</v>
+      </c>
+      <c r="H13" s="5">
+        <f>I13+I10</f>
+        <v>15.319005524314637</v>
+      </c>
+      <c r="I13" s="5">
+        <f>J13+J10</f>
+        <v>11.754979427561166</v>
+      </c>
+      <c r="J13" s="5">
+        <f>K13+K10</f>
+        <v>7.9507533623805511</v>
+      </c>
+      <c r="K13" s="5">
+        <f>L13+L10</f>
+        <v>4</v>
+      </c>
+      <c r="L13" s="5">
         <v>0</v>
       </c>
-      <c r="C10" s="6">
-        <f>COS(81 * PI() / 180) * L10</f>
-        <v>1.877213580482771</v>
-      </c>
-      <c r="D10" s="6">
-        <f>COS(72 * PI() / 180) * L10</f>
-        <v>3.7082039324993694</v>
-      </c>
-      <c r="E10" s="6">
-        <f>COS(63 * PI() / 180) * L10</f>
-        <v>5.4478859968745619</v>
-      </c>
-      <c r="F10" s="6">
-        <f>COS(54 * PI() / 180) * L10</f>
-        <v>7.0534230275096776</v>
-      </c>
-      <c r="G10" s="6">
-        <f>COS(45 * PI() / 180) * L10</f>
-        <v>8.4852813742385713</v>
-      </c>
-      <c r="H10" s="6">
-        <f>COS(36 * PI() / 180) * L10</f>
-        <v>9.7082039324993694</v>
-      </c>
-      <c r="I10" s="6">
-        <f>COS(27 * PI() / 180) * L10</f>
-        <v>10.692078290260415</v>
-      </c>
-      <c r="J10" s="6">
-        <f>COS(18 * PI() / 180) * L10</f>
-        <v>11.412678195541842</v>
-      </c>
-      <c r="K10" s="6">
-        <f>COS(9 * PI() / 180) * L10</f>
-        <v>11.852260087141653</v>
-      </c>
-      <c r="L10" s="6">
-        <f>B6</f>
-        <v>12</v>
+      <c r="R13" s="5"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="13">
+        <f>B12*$F$6+B13*$J$6</f>
+        <v>274.12409472349412</v>
+      </c>
+      <c r="C14" s="13">
+        <f>C12*$F$6+C13*$J$6</f>
+        <v>315.86671612188491</v>
+      </c>
+      <c r="D14" s="13">
+        <f>D12*$F$6+D13*$J$6</f>
+        <v>350.91507669545359</v>
+      </c>
+      <c r="E14" s="13">
+        <f>E12*$F$6+E13*$J$6</f>
+        <v>378.4061694880391</v>
+      </c>
+      <c r="F14" s="13">
+        <f>F12*$F$6+F13*$J$6</f>
+        <v>397.66307255738184</v>
+      </c>
+      <c r="G14" s="13">
+        <f>G12*$F$6+G13*$J$6</f>
+        <v>408.21161703991743</v>
+      </c>
+      <c r="H14" s="13">
+        <f>H12*$F$6+H13*$J$6</f>
+        <v>409.79206276187381</v>
+      </c>
+      <c r="I14" s="13">
+        <f>I12*$F$6+I13*$J$6</f>
+        <v>402.36549390437779</v>
+      </c>
+      <c r="J14" s="13">
+        <f>J12*$F$6+J13*$J$6</f>
+        <v>386.11477724006988</v>
+      </c>
+      <c r="K14" s="13">
+        <f>K12*$F$6+K13*$J$6</f>
+        <v>361.44005934626188</v>
+      </c>
+      <c r="L14" s="13">
+        <f>L12*$F$6+L13*$J$6</f>
+        <v>328.94891366819297</v>
       </c>
     </row>
   </sheetData>
@@ -1810,6 +3026,9 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="H6:I6"/>
   </mergeCells>
+  <conditionalFormatting sqref="B14:L14">
+    <cfRule type="top10" dxfId="0" priority="1" rank="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Changed "cost" to "price" in prompt.
</commit_message>
<xml_diff>
--- a/PPF.xlsx
+++ b/PPF.xlsx
@@ -87,12 +87,6 @@
     <t>Enter Max. Units:</t>
   </si>
   <si>
-    <t>Enter cost of 1 pizza:</t>
-  </si>
-  <si>
-    <t>Enter cost of 1 book:</t>
-  </si>
-  <si>
     <t>Pizza Possibilities:</t>
   </si>
   <si>
@@ -100,6 +94,12 @@
   </si>
   <si>
     <t>Tot. Revenue:</t>
+  </si>
+  <si>
+    <t>Enter price of 1 pizza:</t>
+  </si>
+  <si>
+    <t>Enter price of 1 book:</t>
   </si>
 </sst>
 </file>
@@ -894,34 +894,34 @@
                   <c:v>342.6551184043676</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>394.833395152356</c:v>
+                  <c:v>374.833395152356</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>438.643845869317</c:v>
+                  <c:v>398.8900790574142</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>473.0077118600489</c:v>
+                  <c:v>414.232814722243</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>497.0788406967272</c:v>
+                  <c:v>420.4838130751541</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>510.2645212998967</c:v>
+                  <c:v>417.4891537908246</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>512.2400784523422</c:v>
+                  <c:v>405.3225753195391</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>502.9568673804722</c:v>
+                  <c:v>384.2836592018197</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>482.6434715500873</c:v>
+                  <c:v>354.8904533766438</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>451.8000741828273</c:v>
+                  <c:v>317.8667161218848</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>411.1861420852411</c:v>
+                  <c:v>274.1240947234941</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2675,7 +2675,7 @@
   <dimension ref="A2:R14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2715,14 +2715,14 @@
         <v>5</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="5">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I6" s="13"/>
       <c r="J6" s="6">
@@ -2865,7 +2865,7 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B12" s="3">
         <v>0</v>
@@ -2913,7 +2913,7 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B13" s="3">
         <f t="shared" ref="B13:K13" si="1">C13+C10</f>
@@ -2962,7 +2962,7 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B14" s="9">
         <f t="shared" ref="B14:L14" si="2">B12*$F$6+B13*$J$6</f>
@@ -2970,43 +2970,43 @@
       </c>
       <c r="C14" s="9">
         <f t="shared" si="2"/>
-        <v>394.83339515235605</v>
+        <v>374.83339515235605</v>
       </c>
       <c r="D14" s="9">
         <f t="shared" si="2"/>
-        <v>438.64384586931698</v>
+        <v>398.8900790574142</v>
       </c>
       <c r="E14" s="9">
         <f t="shared" si="2"/>
-        <v>473.00771186004886</v>
+        <v>414.23281472224301</v>
       </c>
       <c r="F14" s="9">
         <f t="shared" si="2"/>
-        <v>497.07884069672724</v>
+        <v>420.4838130751541</v>
       </c>
       <c r="G14" s="9">
         <f t="shared" si="2"/>
-        <v>510.26452129989673</v>
+        <v>417.48915379082456</v>
       </c>
       <c r="H14" s="9">
         <f t="shared" si="2"/>
-        <v>512.24007845234223</v>
+        <v>405.32257531953911</v>
       </c>
       <c r="I14" s="9">
         <f t="shared" si="2"/>
-        <v>502.9568673804722</v>
+        <v>384.28365920181966</v>
       </c>
       <c r="J14" s="9">
         <f t="shared" si="2"/>
-        <v>482.64347155008733</v>
+        <v>354.89045337664385</v>
       </c>
       <c r="K14" s="9">
         <f t="shared" si="2"/>
-        <v>451.8000741828273</v>
+        <v>317.86671612188485</v>
       </c>
       <c r="L14" s="9">
         <f t="shared" si="2"/>
-        <v>411.1861420852411</v>
+        <v>274.12409472349407</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Highlight best revenue point on chart
The spreadsheet now highlights the optimum revenue point along the PPF.
</commit_message>
<xml_diff>
--- a/PPF.xlsx
+++ b/PPF.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="1220" windowWidth="41820" windowHeight="22540" tabRatio="500"/>
+    <workbookView xWindow="5040" yWindow="660" windowWidth="41820" windowHeight="22540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -155,7 +155,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -197,6 +197,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -254,7 +260,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="5" applyAlignment="1">
@@ -283,6 +289,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="44" fontId="5" fillId="9" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="40% - Accent6" xfId="8" builtinId="51"/>
@@ -295,7 +302,17 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="2" builtinId="15"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -521,6 +538,76 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Highlight</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent2">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$N$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>29.66830204466314</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$N$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>14.69372428445146</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -529,11 +616,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2115168288"/>
-        <c:axId val="-2115153520"/>
+        <c:axId val="-2118495392"/>
+        <c:axId val="-2118474288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2115168288"/>
+        <c:axId val="-2118495392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="40.0"/>
@@ -628,13 +715,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2115153520"/>
+        <c:crossAx val="-2118474288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="8.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2115153520"/>
+        <c:axId val="-2118474288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="40.0"/>
@@ -732,7 +819,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2115168288"/>
+        <c:crossAx val="-2118495392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="8.0"/>
@@ -894,34 +981,34 @@
                   <c:v>342.6551184043676</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>374.833395152356</c:v>
+                  <c:v>424.833395152356</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>398.8900790574142</c:v>
+                  <c:v>498.2744960871711</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>414.232814722243</c:v>
+                  <c:v>561.1700575667575</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>420.4838130751541</c:v>
+                  <c:v>611.971382129087</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>417.4891537908246</c:v>
+                  <c:v>649.4275725635049</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>405.3225753195391</c:v>
+                  <c:v>672.6163331515467</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>384.2836592018197</c:v>
+                  <c:v>680.9666796484511</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>354.8904533766438</c:v>
+                  <c:v>674.2729988102526</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>317.8667161218848</c:v>
+                  <c:v>652.700111274241</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>274.1240947234941</c:v>
+                  <c:v>616.7792131278616</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -937,11 +1024,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2115059536"/>
-        <c:axId val="-2115053216"/>
+        <c:axId val="-2119148048"/>
+        <c:axId val="-2119154384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2115059536"/>
+        <c:axId val="-2119148048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1056,7 +1143,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2115053216"/>
+        <c:crossAx val="-2119154384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1064,7 +1151,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2115053216"/>
+        <c:axId val="-2119154384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1125,7 +1212,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2115059536"/>
+        <c:crossAx val="-2119148048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2674,8 +2761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2719,7 +2806,7 @@
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="5">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="H6" s="12" t="s">
         <v>21</v>
@@ -2910,6 +2997,10 @@
         <f t="shared" si="0"/>
         <v>34.265511840436758</v>
       </c>
+      <c r="N12" s="3">
+        <f ca="1">OFFSET(INDIRECT(N14), -2, 0)</f>
+        <v>29.668302044663136</v>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
@@ -2957,6 +3048,10 @@
       </c>
       <c r="L13" s="3">
         <v>0</v>
+      </c>
+      <c r="N13">
+        <f ca="1">OFFSET(INDIRECT(N14), -1, 0)</f>
+        <v>14.693724284451456</v>
       </c>
       <c r="R13" s="3"/>
     </row>
@@ -2970,43 +3065,47 @@
       </c>
       <c r="C14" s="9">
         <f t="shared" si="2"/>
-        <v>374.83339515235605</v>
+        <v>424.83339515235605</v>
       </c>
       <c r="D14" s="9">
         <f t="shared" si="2"/>
-        <v>398.8900790574142</v>
+        <v>498.27449608717109</v>
       </c>
       <c r="E14" s="9">
         <f t="shared" si="2"/>
-        <v>414.23281472224301</v>
+        <v>561.17005756675758</v>
       </c>
       <c r="F14" s="9">
         <f t="shared" si="2"/>
-        <v>420.4838130751541</v>
+        <v>611.97138212908703</v>
       </c>
       <c r="G14" s="9">
         <f t="shared" si="2"/>
-        <v>417.48915379082456</v>
+        <v>649.4275725635049</v>
       </c>
       <c r="H14" s="9">
         <f t="shared" si="2"/>
-        <v>405.32257531953911</v>
+        <v>672.61633315154677</v>
       </c>
       <c r="I14" s="9">
         <f t="shared" si="2"/>
-        <v>384.28365920181966</v>
+        <v>680.96667964845108</v>
       </c>
       <c r="J14" s="9">
         <f t="shared" si="2"/>
-        <v>354.89045337664385</v>
+        <v>674.2729988102526</v>
       </c>
       <c r="K14" s="9">
         <f t="shared" si="2"/>
-        <v>317.86671612188485</v>
+        <v>652.70011127424095</v>
       </c>
       <c r="L14" s="9">
         <f t="shared" si="2"/>
-        <v>274.12409472349407</v>
+        <v>616.77921312786168</v>
+      </c>
+      <c r="N14" s="14" t="str">
+        <f ca="1">CELL("address",OFFSET(B14,0,MATCH(MAX(B14:L14),B14:L14,0)-1))</f>
+        <v>$I$14</v>
       </c>
     </row>
   </sheetData>
@@ -3016,8 +3115,8 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="H6:I6"/>
   </mergeCells>
-  <conditionalFormatting sqref="B14:L14">
-    <cfRule type="top10" dxfId="0" priority="1" rank="1"/>
+  <conditionalFormatting sqref="B14:L14 N14">
+    <cfRule type="top10" dxfId="1" priority="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Made revenue-maximizing point larger
Also added bigger glow around it.
</commit_message>
<xml_diff>
--- a/PPF.xlsx
+++ b/PPF.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>La Famiglia Pizzeria and Bookstore</t>
   </si>
@@ -101,6 +101,12 @@
   <si>
     <t>Enter price of 1 book:</t>
   </si>
+  <si>
+    <t>Opt. pizza:</t>
+  </si>
+  <si>
+    <t>Opt. book:</t>
+  </si>
 </sst>
 </file>
 
@@ -109,7 +115,14 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -251,45 +264,45 @@
   </borders>
   <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="4"/>
-    <xf numFmtId="44" fontId="4" fillId="2" borderId="2" xfId="4" applyNumberFormat="1"/>
-    <xf numFmtId="44" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="6" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="4"/>
+    <xf numFmtId="44" fontId="5" fillId="2" borderId="2" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="6" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="7" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="44" fontId="1" fillId="6" borderId="0" xfId="8" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="2" fillId="6" borderId="0" xfId="8" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="7" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="7" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="7" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="9" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="1" fillId="9" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="40% - Accent6" xfId="8" builtinId="51"/>
@@ -547,21 +560,22 @@
           <c:spPr>
             <a:ln w="22225" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent4"/>
               </a:solidFill>
             </a:ln>
             <a:effectLst>
-              <a:glow rad="139700">
+              <a:glow rad="292100">
                 <a:schemeClr val="accent2">
-                  <a:satMod val="175000"/>
-                  <a:alpha val="14000"/>
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                  <a:alpha val="24000"/>
                 </a:schemeClr>
               </a:glow>
             </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="3"/>
+            <c:size val="6"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent2">
@@ -573,10 +587,11 @@
                 <a:noFill/>
               </a:ln>
               <a:effectLst>
-                <a:glow rad="63500">
+                <a:glow rad="292100">
                   <a:schemeClr val="accent2">
-                    <a:satMod val="175000"/>
-                    <a:alpha val="25000"/>
+                    <a:lumMod val="20000"/>
+                    <a:lumOff val="80000"/>
+                    <a:alpha val="24000"/>
                   </a:schemeClr>
                 </a:glow>
               </a:effectLst>
@@ -589,7 +604,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>29.66830204466314</c:v>
+                  <c:v>9.938441702975689</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -601,7 +616,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>14.69372428445146</c:v>
+                  <c:v>31.93825454336087</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -981,34 +996,34 @@
                   <c:v>342.6551184043676</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>424.833395152356</c:v>
+                  <c:v>354.833395152356</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>498.2744960871711</c:v>
+                  <c:v>359.1363122455115</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>561.1700575667575</c:v>
+                  <c:v>355.4579175844372</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>611.971382129087</c:v>
+                  <c:v>343.8887854535809</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>649.4275725635049</c:v>
+                  <c:v>324.7137862817524</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>672.6163331515467</c:v>
+                  <c:v>298.405072186736</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>680.9666796484511</c:v>
+                  <c:v>265.6104510231671</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>674.2729988102526</c:v>
+                  <c:v>227.1374352032004</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>652.700111274241</c:v>
+                  <c:v>183.9333580609424</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>616.7792131278616</c:v>
+                  <c:v>137.062047361747</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2761,8 +2776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2806,7 +2821,7 @@
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="5">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="H6" s="12" t="s">
         <v>21</v>
@@ -2997,9 +3012,12 @@
         <f t="shared" si="0"/>
         <v>34.265511840436758</v>
       </c>
+      <c r="M12" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="N12" s="3">
         <f ca="1">OFFSET(INDIRECT(N14), -2, 0)</f>
-        <v>29.668302044663136</v>
+        <v>9.9384417029756893</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
@@ -3049,9 +3067,12 @@
       <c r="L13" s="3">
         <v>0</v>
       </c>
+      <c r="M13" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="N13">
         <f ca="1">OFFSET(INDIRECT(N14), -1, 0)</f>
-        <v>14.693724284451456</v>
+        <v>31.93825454336087</v>
       </c>
       <c r="R13" s="3"/>
     </row>
@@ -3065,47 +3086,47 @@
       </c>
       <c r="C14" s="9">
         <f t="shared" si="2"/>
-        <v>424.83339515235605</v>
+        <v>354.83339515235605</v>
       </c>
       <c r="D14" s="9">
         <f t="shared" si="2"/>
-        <v>498.27449608717109</v>
+        <v>359.13631224551148</v>
       </c>
       <c r="E14" s="9">
         <f t="shared" si="2"/>
-        <v>561.17005756675758</v>
+        <v>355.45791758443715</v>
       </c>
       <c r="F14" s="9">
         <f t="shared" si="2"/>
-        <v>611.97138212908703</v>
+        <v>343.88878545358091</v>
       </c>
       <c r="G14" s="9">
         <f t="shared" si="2"/>
-        <v>649.4275725635049</v>
+        <v>324.71378628175245</v>
       </c>
       <c r="H14" s="9">
         <f t="shared" si="2"/>
-        <v>672.61633315154677</v>
+        <v>298.40507218673605</v>
       </c>
       <c r="I14" s="9">
         <f t="shared" si="2"/>
-        <v>680.96667964845108</v>
+        <v>265.61045102316712</v>
       </c>
       <c r="J14" s="9">
         <f t="shared" si="2"/>
-        <v>674.2729988102526</v>
+        <v>227.13743520320037</v>
       </c>
       <c r="K14" s="9">
         <f t="shared" si="2"/>
-        <v>652.70011127424095</v>
+        <v>183.93335806094242</v>
       </c>
       <c r="L14" s="9">
         <f t="shared" si="2"/>
-        <v>616.77921312786168</v>
+        <v>137.06204736174703</v>
       </c>
       <c r="N14" s="14" t="str">
         <f ca="1">CELL("address",OFFSET(B14,0,MATCH(MAX(B14:L14),B14:L14,0)-1))</f>
-        <v>$I$14</v>
+        <v>$D$14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added supply and demand model.
</commit_message>
<xml_diff>
--- a/PPF.xlsx
+++ b/PPF.xlsx
@@ -604,7 +604,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>9.938441702975689</c:v>
+                  <c:v>33.48333951523561</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -613,10 +613,10 @@
             <c:numRef>
               <c:f>Sheet1!$N$13</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>31.93825454336087</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -996,34 +996,34 @@
                   <c:v>342.6551184043676</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>354.833395152356</c:v>
+                  <c:v>534.833395152356</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>359.1363122455115</c:v>
+                  <c:v>716.9202135526362</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>355.4579175844372</c:v>
+                  <c:v>884.4319918246897</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>343.8887854535809</c:v>
+                  <c:v>1033.24403404774</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>324.7137862817524</c:v>
+                  <c:v>1159.692093863402</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>298.405072186736</c:v>
+                  <c:v>1260.662600381964</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>265.6104510231671</c:v>
+                  <c:v>1333.66932463104</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>227.1374352032004</c:v>
+                  <c:v>1376.914598764192</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>183.9333580609424</c:v>
+                  <c:v>1389.333580609424</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>137.062047361747</c:v>
+                  <c:v>1370.62047361747</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2821,7 +2821,7 @@
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="5">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="H6" s="12" t="s">
         <v>21</v>
@@ -3017,7 +3017,7 @@
       </c>
       <c r="N12" s="3">
         <f ca="1">OFFSET(INDIRECT(N14), -2, 0)</f>
-        <v>9.9384417029756893</v>
+        <v>33.483339515235606</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
@@ -3070,9 +3070,9 @@
       <c r="M13" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="N13">
+      <c r="N13" s="3">
         <f ca="1">OFFSET(INDIRECT(N14), -1, 0)</f>
-        <v>31.93825454336087</v>
+        <v>5</v>
       </c>
       <c r="R13" s="3"/>
     </row>
@@ -3086,47 +3086,47 @@
       </c>
       <c r="C14" s="9">
         <f t="shared" si="2"/>
-        <v>354.83339515235605</v>
+        <v>534.83339515235605</v>
       </c>
       <c r="D14" s="9">
         <f t="shared" si="2"/>
-        <v>359.13631224551148</v>
+        <v>716.92021355263626</v>
       </c>
       <c r="E14" s="9">
         <f t="shared" si="2"/>
-        <v>355.45791758443715</v>
+        <v>884.4319918246897</v>
       </c>
       <c r="F14" s="9">
         <f t="shared" si="2"/>
-        <v>343.88878545358091</v>
+        <v>1033.2440340477397</v>
       </c>
       <c r="G14" s="9">
         <f t="shared" si="2"/>
-        <v>324.71378628175245</v>
+        <v>1159.6920938634016</v>
       </c>
       <c r="H14" s="9">
         <f t="shared" si="2"/>
-        <v>298.40507218673605</v>
+        <v>1260.6626003819638</v>
       </c>
       <c r="I14" s="9">
         <f t="shared" si="2"/>
-        <v>265.61045102316712</v>
+        <v>1333.6693246310401</v>
       </c>
       <c r="J14" s="9">
         <f t="shared" si="2"/>
-        <v>227.13743520320037</v>
+        <v>1376.9145987641916</v>
       </c>
       <c r="K14" s="9">
         <f t="shared" si="2"/>
-        <v>183.93335806094242</v>
+        <v>1389.3335806094242</v>
       </c>
       <c r="L14" s="9">
         <f t="shared" si="2"/>
-        <v>137.06204736174703</v>
+        <v>1370.6204736174705</v>
       </c>
       <c r="N14" s="14" t="str">
         <f ca="1">CELL("address",OFFSET(B14,0,MATCH(MAX(B14:L14),B14:L14,0)-1))</f>
-        <v>$D$14</v>
+        <v>$K$14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>